<commit_message>
modify aug pc results
</commit_message>
<xml_diff>
--- a/aug_pc_result/2026_Feb_06_11_23_22_d_separation_kci_pc_gt_graph_AdaSyn_20_3001859/results.xlsx
+++ b/aug_pc_result/2026_Feb_06_11_23_22_d_separation_kci_pc_gt_graph_AdaSyn_20_3001859/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CausalLearning\code\aug_pc_result\2026_Feb_06_11_23_22_d_separation_kci_pc_gt_graph_AdaSyn_20_3001859\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4BB764-B7C8-437A-A8FA-FB9E26281BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32D2FA6-EC69-429F-A0C6-9F248066EC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>

</xml_diff>